<commit_message>
Modified EXDC1 to calculate Ae, Be from E1, E2, SE1 and SE2.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_aw.xlsx
+++ b/andes/cases/kundur/kundur_aw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/Nextcloud/notebooks/kundur/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F84E1C5-9C85-0B49-8211-8B485AE7184F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5BD323-73F5-754B-81D2-A475C0EFC274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="6300" windowWidth="28880" windowHeight="19340" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10900" yWindow="1800" windowWidth="28880" windowHeight="19340" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
   <si>
     <t>idx</t>
   </si>
@@ -314,12 +314,6 @@
   </si>
   <si>
     <t>TGOV1_1</t>
-  </si>
-  <si>
-    <t>Ae</t>
-  </si>
-  <si>
-    <t>Be</t>
   </si>
   <si>
     <t>EXDC2_1</t>
@@ -392,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,13 +398,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -462,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -470,7 +457,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3368,7 +3354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3394,10 +3380,10 @@
         <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I1" t="s">
         <v>91</v>
@@ -3409,7 +3395,7 @@
         <v>93</v>
       </c>
       <c r="L1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3571,16 +3557,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3597,43 +3583,43 @@
         <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>113</v>
@@ -3641,14 +3627,8 @@
       <c r="T1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3659,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3709,14 +3689,8 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2" s="3">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3727,7 +3701,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3777,14 +3751,8 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3" s="3">
-        <v>0</v>
-      </c>
-      <c r="V3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3795,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3845,14 +3813,8 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3863,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3911,12 +3873,6 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated EXDC2 to quadratic saturation; Updated all cases; reverted inplace assignment for jacobian values.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_aw.xlsx
+++ b/andes/cases/kundur/kundur_aw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5BD323-73F5-754B-81D2-A475C0EFC274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910F3A3E-EB6C-3943-83B8-B2E13544BED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10900" yWindow="1800" windowWidth="28880" windowHeight="19340" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3561,7 +3561,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6:T6"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3684,10 +3684,10 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -3746,10 +3746,10 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -3808,10 +3808,10 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -3870,10 +3870,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>